<commit_message>
Computer Management | 修复Socket不执行Loading函数的情况 | 添加ComputerUI | 添加Web服务器
Weteoes_C Model
| 修复IO_ReadFile 读取文件不全的情况
</commit_message>
<xml_diff>
--- a/Computer Management Project/Weteoes/Software.xlsx
+++ b/Computer Management Project/Weteoes/Software.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D67E9F-ED91-48B8-B55B-560E34FB3724}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BA39BC-ED5D-4774-91D2-5AA8F5659BF7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="2595" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8535" yWindow="6600" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exit Code" sheetId="1" r:id="rId1"/>
     <sheet name="依赖性" sheetId="2" r:id="rId2"/>
+    <sheet name="端口" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>CComputerApp::Loading</t>
   </si>
@@ -106,6 +107,18 @@
   </si>
   <si>
     <t>libcrypto-1_1-x64.dll, Dll_Client, Dll_Management</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ComputerUI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Control</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用于进程间通讯</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -162,14 +175,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -593,7 +615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2586BE86-0FEC-4A29-985C-A9C95E84BB7F}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -658,28 +680,77 @@
       <c r="H5" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A7:H7"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B5:H5"/>
-    <mergeCell ref="A7:H7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1127762D-566F-4FCE-BFCA-BD6C60A77DDF}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2">
+        <v>23332</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="5">
+        <v>23333</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>